<commit_message>
Added four new metrics for strings (min/max for case sensitive/insensitive - using lexical order)
</commit_message>
<xml_diff>
--- a/docs/profiler-metric-mapping.xlsx
+++ b/docs/profiler-metric-mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="48">
   <si>
     <t>MIN_TIMESTAMP</t>
   </si>
@@ -151,6 +151,18 @@
   </si>
   <si>
     <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>MAX_STRING_CASE</t>
+  </si>
+  <si>
+    <t>MIN_STRING_CASE</t>
+  </si>
+  <si>
+    <t>MAX_STRING_ICASE</t>
+  </si>
+  <si>
+    <t>MIN_STRING_ICASE</t>
   </si>
 </sst>
 </file>
@@ -253,8 +265,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -310,7 +324,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -332,6 +346,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -353,6 +368,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -682,7 +698,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
@@ -1301,129 +1317,91 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>41</v>
@@ -1443,7 +1421,9 @@
       <c r="G23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1452,7 +1432,7 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>41</v>
@@ -1472,7 +1452,9 @@
       <c r="G24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1481,83 +1463,125 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
-      <c r="K26" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1568,15 +1592,15 @@
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="K29" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="L29" s="3"/>
-      <c r="M29" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="M29" s="3"/>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1587,9 +1611,85 @@
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
+      <c r="K30" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="L30" s="3"/>
-      <c r="M30" s="3" t="s">
+      <c r="M30" s="3"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M32" s="3"/>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>